<commit_message>
Add SPAR technical areas and indicators to the data dictionary
</commit_message>
<xml_diff>
--- a/data/Data Dictionary.xlsx
+++ b/data/Data Dictionary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="338">
   <si>
     <r>
       <rPr>
@@ -1974,6 +1974,78 @@
     </r>
   </si>
   <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>IHR Coordination and National IHR Focal Point Functions</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>Zoonotic events and the human-animal interface</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>Food safety</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>Laboratory</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>Surveillance</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>Human resources</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>National health emergency framework</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>Health service provision</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>Risk communication</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>Points of entry</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>Chemical events</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>Radiation emergencies</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -2014,6 +2086,138 @@
     </r>
   </si>
   <si>
+    <t>Financing for the implementation of IHR capacities</t>
+  </si>
+  <si>
+    <t>Financing mechanism and funds for timely response to public health emergencies</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>National IHR Focal Point functions under IHR</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>Multisectoral IHR coordination mechanisms</t>
+  </si>
+  <si>
+    <t>C31</t>
+  </si>
+  <si>
+    <t>Collaborative effort on activities to address zoonoses</t>
+  </si>
+  <si>
+    <t>C41</t>
+  </si>
+  <si>
+    <t>Multisectoral collaboration mechanism for food safety events</t>
+  </si>
+  <si>
+    <t>C51</t>
+  </si>
+  <si>
+    <t>Specimen referral and transport system</t>
+  </si>
+  <si>
+    <t>C52</t>
+  </si>
+  <si>
+    <t>Implementation of a laboratory biosafety and biosecurity regime</t>
+  </si>
+  <si>
+    <t>C53</t>
+  </si>
+  <si>
+    <t>Access to laboratory testing capacity for priority diseases</t>
+  </si>
+  <si>
+    <t>C61</t>
+  </si>
+  <si>
+    <t>Early warning function: indicator- and event-based surveillance</t>
+  </si>
+  <si>
+    <t>C62</t>
+  </si>
+  <si>
+    <t>Mechanism for event management (verification, risk assessment, analysis invesgitation)</t>
+  </si>
+  <si>
+    <t>C71</t>
+  </si>
+  <si>
+    <t>Human resources for implementation of IHR capacities</t>
+  </si>
+  <si>
+    <t>C81</t>
+  </si>
+  <si>
+    <t>Planning for emergency preparedness and response mechanism</t>
+  </si>
+  <si>
+    <t>C82</t>
+  </si>
+  <si>
+    <t>Management of health emergency response operations</t>
+  </si>
+  <si>
+    <t>C83</t>
+  </si>
+  <si>
+    <t>Emergency resource mobilization</t>
+  </si>
+  <si>
+    <t>C91</t>
+  </si>
+  <si>
+    <t>Case management capacity for IHR relevant hazards</t>
+  </si>
+  <si>
+    <t>C92</t>
+  </si>
+  <si>
+    <t>Capacity for infection prevention and control and chemical and radiation decontamination</t>
+  </si>
+  <si>
+    <t>C93</t>
+  </si>
+  <si>
+    <t>Access to essential health services</t>
+  </si>
+  <si>
+    <t>C101</t>
+  </si>
+  <si>
+    <t>Capacity for emergency risk communications</t>
+  </si>
+  <si>
+    <t>C111</t>
+  </si>
+  <si>
+    <t>Core capacity requirements at all times for designated airports, ports and ground crossings</t>
+  </si>
+  <si>
+    <t>C112</t>
+  </si>
+  <si>
+    <t>Effective public health response at points of entry</t>
+  </si>
+  <si>
+    <t>C121</t>
+  </si>
+  <si>
+    <t>Resources for detection and alert</t>
+  </si>
+  <si>
+    <t>C131</t>
+  </si>
+  <si>
+    <t>Capacity and resources</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -2110,15 +2314,7 @@
         <color indexed="8"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>Domestic legislation, laws, regulations, policy and administrative requirements are available in all relevant</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">
+      <t xml:space="preserve">Domestic legislation, laws, regulations, policy and administrative requirements are available in all relevant
 </t>
     </r>
     <r>
@@ -2137,15 +2333,7 @@
         <color indexed="8"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>Benchmark</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">
+      <t xml:space="preserve">Benchmark
 </t>
     </r>
     <r>
@@ -2174,15 +2362,7 @@
         <color indexed="8"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>To assess, adjust and align domestic legislation, laws, regulations, policy and administrative requirements in all</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">
+      <t xml:space="preserve">To assess, adjust and align domestic legislation, laws, regulations, policy and administrative requirements in all
 </t>
     </r>
     <r>
@@ -2351,15 +2531,7 @@
         <color indexed="8"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">
+      <t xml:space="preserve">1
 </t>
     </r>
   </si>
@@ -2812,12 +2984,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -2827,61 +2999,128 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
-      <bottom>
-        <color indexed="8"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
-      <top>
-        <color indexed="8"/>
+      <top style="thin">
+        <color indexed="10"/>
       </top>
-      <bottom>
-        <color indexed="8"/>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="11"/>
       </right>
-      <top>
-        <color indexed="8"/>
+      <top style="thin">
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2891,33 +3130,51 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2936,8 +3193,9 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff7f7f7f"/>
-      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffc0c0c0"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -2948,15 +3206,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1229906</xdr:colOff>
+      <xdr:colOff>1210856</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>348541</xdr:rowOff>
+      <xdr:rowOff>329488</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>264706</xdr:colOff>
+      <xdr:colOff>245656</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>640641</xdr:rowOff>
+      <xdr:rowOff>621588</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2965,7 +3223,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11186706" y="39904596"/>
+          <a:off x="11167656" y="39885543"/>
           <a:ext cx="1524001" cy="292101"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4109,7 +4367,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K186"/>
+  <dimension ref="A1:K212"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -6501,8 +6759,12 @@
       <c r="B138" s="7"/>
       <c r="C138" s="7"/>
       <c r="D138" s="7"/>
-      <c r="E138" s="7"/>
-      <c r="F138" s="7"/>
+      <c r="E138" t="s" s="9">
+        <v>196</v>
+      </c>
+      <c r="F138" t="s" s="9">
+        <v>197</v>
+      </c>
       <c r="G138" s="7"/>
       <c r="H138" s="7"/>
       <c r="I138" s="7"/>
@@ -6514,8 +6776,12 @@
       <c r="B139" s="7"/>
       <c r="C139" s="7"/>
       <c r="D139" s="7"/>
-      <c r="E139" s="7"/>
-      <c r="F139" s="7"/>
+      <c r="E139" t="s" s="9">
+        <v>198</v>
+      </c>
+      <c r="F139" t="s" s="9">
+        <v>199</v>
+      </c>
       <c r="G139" s="7"/>
       <c r="H139" s="7"/>
       <c r="I139" s="7"/>
@@ -6527,8 +6793,12 @@
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
       <c r="D140" s="7"/>
-      <c r="E140" s="7"/>
-      <c r="F140" s="7"/>
+      <c r="E140" t="s" s="9">
+        <v>200</v>
+      </c>
+      <c r="F140" t="s" s="9">
+        <v>201</v>
+      </c>
       <c r="G140" s="7"/>
       <c r="H140" s="7"/>
       <c r="I140" s="7"/>
@@ -6540,8 +6810,12 @@
       <c r="B141" s="7"/>
       <c r="C141" s="7"/>
       <c r="D141" s="7"/>
-      <c r="E141" s="7"/>
-      <c r="F141" s="7"/>
+      <c r="E141" t="s" s="9">
+        <v>202</v>
+      </c>
+      <c r="F141" t="s" s="9">
+        <v>203</v>
+      </c>
       <c r="G141" s="7"/>
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
@@ -6553,46 +6827,46 @@
       <c r="B142" s="7"/>
       <c r="C142" s="7"/>
       <c r="D142" s="7"/>
-      <c r="E142" s="7"/>
-      <c r="F142" s="7"/>
+      <c r="E142" t="s" s="9">
+        <v>204</v>
+      </c>
+      <c r="F142" t="s" s="9">
+        <v>205</v>
+      </c>
       <c r="G142" s="7"/>
       <c r="H142" s="7"/>
       <c r="I142" s="7"/>
       <c r="J142" s="7"/>
       <c r="K142" s="7"/>
     </row>
-    <row r="143" ht="116.5" customHeight="1">
-      <c r="A143" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="B143" t="s" s="2">
-        <v>192</v>
-      </c>
-      <c r="C143" t="s" s="2">
-        <v>197</v>
-      </c>
-      <c r="D143" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="E143" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="F143" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="G143" s="3"/>
-      <c r="H143" s="3"/>
-      <c r="I143" s="3"/>
-      <c r="J143" s="3"/>
-      <c r="K143" s="3"/>
+    <row r="143" ht="20.5" customHeight="1">
+      <c r="A143" s="7"/>
+      <c r="B143" s="7"/>
+      <c r="C143" s="7"/>
+      <c r="D143" s="7"/>
+      <c r="E143" t="s" s="9">
+        <v>206</v>
+      </c>
+      <c r="F143" t="s" s="9">
+        <v>207</v>
+      </c>
+      <c r="G143" s="7"/>
+      <c r="H143" s="7"/>
+      <c r="I143" s="7"/>
+      <c r="J143" s="7"/>
+      <c r="K143" s="7"/>
     </row>
     <row r="144" ht="20.5" customHeight="1">
       <c r="A144" s="7"/>
       <c r="B144" s="7"/>
       <c r="C144" s="7"/>
       <c r="D144" s="7"/>
-      <c r="E144" s="7"/>
-      <c r="F144" s="7"/>
+      <c r="E144" t="s" s="9">
+        <v>208</v>
+      </c>
+      <c r="F144" t="s" s="9">
+        <v>209</v>
+      </c>
       <c r="G144" s="7"/>
       <c r="H144" s="7"/>
       <c r="I144" s="7"/>
@@ -6604,8 +6878,12 @@
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
       <c r="D145" s="7"/>
-      <c r="E145" s="7"/>
-      <c r="F145" s="7"/>
+      <c r="E145" t="s" s="9">
+        <v>210</v>
+      </c>
+      <c r="F145" t="s" s="9">
+        <v>211</v>
+      </c>
       <c r="G145" s="7"/>
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
@@ -6617,8 +6895,12 @@
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
       <c r="D146" s="7"/>
-      <c r="E146" s="7"/>
-      <c r="F146" s="7"/>
+      <c r="E146" t="s" s="9">
+        <v>212</v>
+      </c>
+      <c r="F146" t="s" s="9">
+        <v>213</v>
+      </c>
       <c r="G146" s="7"/>
       <c r="H146" s="7"/>
       <c r="I146" s="7"/>
@@ -6630,8 +6912,12 @@
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
       <c r="D147" s="7"/>
-      <c r="E147" s="7"/>
-      <c r="F147" s="7"/>
+      <c r="E147" t="s" s="9">
+        <v>214</v>
+      </c>
+      <c r="F147" t="s" s="9">
+        <v>215</v>
+      </c>
       <c r="G147" s="7"/>
       <c r="H147" s="7"/>
       <c r="I147" s="7"/>
@@ -6643,8 +6929,12 @@
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
       <c r="D148" s="7"/>
-      <c r="E148" s="7"/>
-      <c r="F148" s="7"/>
+      <c r="E148" t="s" s="9">
+        <v>216</v>
+      </c>
+      <c r="F148" t="s" s="9">
+        <v>217</v>
+      </c>
       <c r="G148" s="7"/>
       <c r="H148" s="7"/>
       <c r="I148" s="7"/>
@@ -6656,87 +6946,85 @@
       <c r="B149" s="7"/>
       <c r="C149" s="7"/>
       <c r="D149" s="7"/>
-      <c r="E149" s="7"/>
-      <c r="F149" s="7"/>
+      <c r="E149" t="s" s="9">
+        <v>218</v>
+      </c>
+      <c r="F149" t="s" s="9">
+        <v>219</v>
+      </c>
       <c r="G149" s="7"/>
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
       <c r="J149" s="7"/>
       <c r="K149" s="7"/>
     </row>
-    <row r="150" ht="44.5" customHeight="1">
-      <c r="A150" t="s" s="2">
-        <v>200</v>
-      </c>
-      <c r="B150" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="C150" t="s" s="2">
-        <v>202</v>
-      </c>
-      <c r="D150" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="E150" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="F150" t="s" s="2">
-        <v>205</v>
-      </c>
-      <c r="G150" s="3"/>
-      <c r="H150" s="3"/>
-      <c r="I150" s="3"/>
-      <c r="J150" s="3"/>
-      <c r="K150" s="3"/>
-    </row>
-    <row r="151" ht="20.5" customHeight="1">
-      <c r="A151" s="7"/>
-      <c r="B151" s="7"/>
-      <c r="C151" s="7"/>
-      <c r="D151" s="7"/>
+    <row r="150" ht="20.5" customHeight="1">
+      <c r="A150" s="7"/>
+      <c r="B150" s="7"/>
+      <c r="C150" s="7"/>
+      <c r="D150" s="7"/>
+      <c r="E150" s="7"/>
+      <c r="F150" s="7"/>
+      <c r="G150" s="7"/>
+      <c r="H150" s="7"/>
+      <c r="I150" s="7"/>
+      <c r="J150" s="7"/>
+      <c r="K150" s="7"/>
+    </row>
+    <row r="151" ht="116.5" customHeight="1">
+      <c r="A151" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="B151" t="s" s="2">
+        <v>192</v>
+      </c>
+      <c r="C151" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="D151" t="s" s="2">
+        <v>9</v>
+      </c>
       <c r="E151" t="s" s="2">
-        <v>206</v>
-      </c>
-      <c r="F151" s="7"/>
-      <c r="G151" s="7"/>
-      <c r="H151" s="7"/>
-      <c r="I151" s="7"/>
-      <c r="J151" s="7"/>
+        <v>222</v>
+      </c>
+      <c r="F151" t="s" s="10">
+        <v>223</v>
+      </c>
+      <c r="G151" s="3"/>
+      <c r="H151" s="3"/>
+      <c r="I151" s="3"/>
+      <c r="J151" s="3"/>
       <c r="K151" s="3"/>
     </row>
-    <row r="152" ht="164.5" customHeight="1">
-      <c r="A152" t="s" s="2">
-        <v>207</v>
-      </c>
-      <c r="B152" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="C152" t="s" s="2">
-        <v>208</v>
-      </c>
-      <c r="D152" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="E152" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="F152" t="s" s="2">
-        <v>209</v>
-      </c>
-      <c r="G152" s="3"/>
-      <c r="H152" s="3"/>
-      <c r="I152" s="3"/>
-      <c r="J152" s="3"/>
-      <c r="K152" s="3"/>
+    <row r="152" ht="20.5" customHeight="1">
+      <c r="A152" s="7"/>
+      <c r="B152" s="7"/>
+      <c r="C152" s="7"/>
+      <c r="D152" s="7"/>
+      <c r="E152" t="s" s="11">
+        <v>216</v>
+      </c>
+      <c r="F152" t="s" s="12">
+        <v>224</v>
+      </c>
+      <c r="G152" s="13"/>
+      <c r="H152" s="7"/>
+      <c r="I152" s="7"/>
+      <c r="J152" s="7"/>
+      <c r="K152" s="7"/>
     </row>
     <row r="153" ht="20.5" customHeight="1">
       <c r="A153" s="7"/>
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
       <c r="D153" s="7"/>
-      <c r="E153" s="7"/>
-      <c r="F153" s="7"/>
-      <c r="G153" s="7"/>
+      <c r="E153" t="s" s="11">
+        <v>218</v>
+      </c>
+      <c r="F153" t="s" s="12">
+        <v>225</v>
+      </c>
+      <c r="G153" s="13"/>
       <c r="H153" s="7"/>
       <c r="I153" s="7"/>
       <c r="J153" s="7"/>
@@ -6747,461 +7035,435 @@
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
       <c r="D154" s="7"/>
-      <c r="E154" s="7"/>
-      <c r="F154" s="7"/>
-      <c r="G154" s="7"/>
+      <c r="E154" t="s" s="11">
+        <v>226</v>
+      </c>
+      <c r="F154" t="s" s="12">
+        <v>227</v>
+      </c>
+      <c r="G154" s="13"/>
       <c r="H154" s="7"/>
       <c r="I154" s="7"/>
       <c r="J154" s="7"/>
       <c r="K154" s="7"/>
     </row>
-    <row r="155" ht="164.5" customHeight="1">
-      <c r="A155" t="s" s="2">
-        <v>210</v>
-      </c>
-      <c r="B155" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="C155" t="s" s="2">
-        <v>211</v>
-      </c>
-      <c r="D155" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="E155" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="F155" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="G155" s="3"/>
-      <c r="H155" s="3"/>
-      <c r="I155" s="3"/>
-      <c r="J155" s="3"/>
-      <c r="K155" s="3"/>
+    <row r="155" ht="20.5" customHeight="1">
+      <c r="A155" s="7"/>
+      <c r="B155" s="7"/>
+      <c r="C155" s="7"/>
+      <c r="D155" s="7"/>
+      <c r="E155" t="s" s="11">
+        <v>228</v>
+      </c>
+      <c r="F155" t="s" s="12">
+        <v>229</v>
+      </c>
+      <c r="G155" s="13"/>
+      <c r="H155" s="7"/>
+      <c r="I155" s="7"/>
+      <c r="J155" s="7"/>
+      <c r="K155" s="7"/>
     </row>
     <row r="156" ht="20.5" customHeight="1">
       <c r="A156" s="7"/>
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
       <c r="D156" s="7"/>
-      <c r="E156" s="7"/>
-      <c r="F156" s="7"/>
-      <c r="G156" s="7"/>
+      <c r="E156" t="s" s="11">
+        <v>230</v>
+      </c>
+      <c r="F156" t="s" s="12">
+        <v>231</v>
+      </c>
+      <c r="G156" s="13"/>
       <c r="H156" s="7"/>
       <c r="I156" s="7"/>
       <c r="J156" s="7"/>
       <c r="K156" s="7"/>
     </row>
     <row r="157" ht="20.5" customHeight="1">
-      <c r="A157" t="s" s="2">
-        <v>213</v>
-      </c>
-      <c r="B157" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="C157" t="s" s="2">
-        <v>214</v>
-      </c>
-      <c r="D157" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="E157" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="F157" t="s" s="2">
-        <v>215</v>
-      </c>
-      <c r="G157" s="3"/>
-      <c r="H157" s="3"/>
-      <c r="I157" s="3"/>
-      <c r="J157" s="3"/>
-      <c r="K157" s="3"/>
+      <c r="A157" s="7"/>
+      <c r="B157" s="7"/>
+      <c r="C157" s="7"/>
+      <c r="D157" s="7"/>
+      <c r="E157" t="s" s="11">
+        <v>232</v>
+      </c>
+      <c r="F157" t="s" s="12">
+        <v>233</v>
+      </c>
+      <c r="G157" s="13"/>
+      <c r="H157" s="7"/>
+      <c r="I157" s="7"/>
+      <c r="J157" s="7"/>
+      <c r="K157" s="7"/>
     </row>
     <row r="158" ht="20.5" customHeight="1">
       <c r="A158" s="7"/>
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
       <c r="D158" s="7"/>
-      <c r="E158" t="s" s="2">
-        <v>206</v>
-      </c>
-      <c r="F158" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="G158" s="7"/>
+      <c r="E158" t="s" s="11">
+        <v>234</v>
+      </c>
+      <c r="F158" t="s" s="12">
+        <v>235</v>
+      </c>
+      <c r="G158" s="13"/>
       <c r="H158" s="7"/>
       <c r="I158" s="7"/>
       <c r="J158" s="7"/>
-      <c r="K158" s="3"/>
+      <c r="K158" s="7"/>
     </row>
     <row r="159" ht="20.5" customHeight="1">
-      <c r="A159" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="B159" t="s" s="2">
-        <v>218</v>
-      </c>
-      <c r="C159" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="D159" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="E159" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="F159" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="G159" s="3"/>
-      <c r="H159" s="3"/>
-      <c r="I159" s="3"/>
-      <c r="J159" s="3"/>
-      <c r="K159" s="3"/>
-    </row>
-    <row r="160" ht="116.5" customHeight="1">
-      <c r="A160" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="B160" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="C160" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="D160" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="E160" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="F160" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="G160" s="3"/>
-      <c r="H160" s="3"/>
-      <c r="I160" s="3"/>
-      <c r="J160" s="3"/>
-      <c r="K160" s="3"/>
-    </row>
-    <row r="161" ht="32.5" customHeight="1">
-      <c r="A161" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="B161" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="C161" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="D161" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="E161" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="F161" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="G161" s="3"/>
-      <c r="H161" s="3"/>
-      <c r="I161" s="3"/>
-      <c r="J161" s="3"/>
-      <c r="K161" s="3"/>
-    </row>
-    <row r="162" ht="32.5" customHeight="1">
+      <c r="A159" s="7"/>
+      <c r="B159" s="7"/>
+      <c r="C159" s="7"/>
+      <c r="D159" s="7"/>
+      <c r="E159" t="s" s="11">
+        <v>236</v>
+      </c>
+      <c r="F159" t="s" s="12">
+        <v>237</v>
+      </c>
+      <c r="G159" s="13"/>
+      <c r="H159" s="7"/>
+      <c r="I159" s="7"/>
+      <c r="J159" s="7"/>
+      <c r="K159" s="7"/>
+    </row>
+    <row r="160" ht="20.5" customHeight="1">
+      <c r="A160" s="7"/>
+      <c r="B160" s="7"/>
+      <c r="C160" s="7"/>
+      <c r="D160" s="7"/>
+      <c r="E160" t="s" s="11">
+        <v>238</v>
+      </c>
+      <c r="F160" t="s" s="12">
+        <v>239</v>
+      </c>
+      <c r="G160" s="13"/>
+      <c r="H160" s="7"/>
+      <c r="I160" s="7"/>
+      <c r="J160" s="7"/>
+      <c r="K160" s="7"/>
+    </row>
+    <row r="161" ht="20.5" customHeight="1">
+      <c r="A161" s="7"/>
+      <c r="B161" s="7"/>
+      <c r="C161" s="7"/>
+      <c r="D161" s="7"/>
+      <c r="E161" t="s" s="11">
+        <v>240</v>
+      </c>
+      <c r="F161" t="s" s="12">
+        <v>241</v>
+      </c>
+      <c r="G161" s="13"/>
+      <c r="H161" s="7"/>
+      <c r="I161" s="7"/>
+      <c r="J161" s="7"/>
+      <c r="K161" s="7"/>
+    </row>
+    <row r="162" ht="20.5" customHeight="1">
       <c r="A162" s="7"/>
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
       <c r="D162" s="7"/>
-      <c r="E162" t="s" s="2">
-        <v>206</v>
-      </c>
-      <c r="F162" t="s" s="2">
-        <v>230</v>
-      </c>
-      <c r="G162" s="7"/>
+      <c r="E162" t="s" s="11">
+        <v>242</v>
+      </c>
+      <c r="F162" t="s" s="12">
+        <v>243</v>
+      </c>
+      <c r="G162" s="13"/>
       <c r="H162" s="7"/>
       <c r="I162" s="7"/>
       <c r="J162" s="7"/>
-      <c r="K162" s="3"/>
+      <c r="K162" s="7"/>
     </row>
     <row r="163" ht="20.5" customHeight="1">
       <c r="A163" s="7"/>
       <c r="B163" s="7"/>
       <c r="C163" s="7"/>
       <c r="D163" s="7"/>
-      <c r="E163" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="F163" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="G163" s="7"/>
+      <c r="E163" t="s" s="11">
+        <v>244</v>
+      </c>
+      <c r="F163" t="s" s="12">
+        <v>245</v>
+      </c>
+      <c r="G163" s="13"/>
       <c r="H163" s="7"/>
       <c r="I163" s="7"/>
       <c r="J163" s="7"/>
-      <c r="K163" s="3"/>
+      <c r="K163" s="7"/>
     </row>
     <row r="164" ht="20.5" customHeight="1">
       <c r="A164" s="7"/>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
       <c r="D164" s="7"/>
-      <c r="E164" t="s" s="2">
-        <v>233</v>
-      </c>
-      <c r="F164" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="G164" s="7"/>
+      <c r="E164" t="s" s="11">
+        <v>246</v>
+      </c>
+      <c r="F164" t="s" s="12">
+        <v>247</v>
+      </c>
+      <c r="G164" s="13"/>
       <c r="H164" s="7"/>
       <c r="I164" s="7"/>
       <c r="J164" s="7"/>
-      <c r="K164" s="3"/>
+      <c r="K164" s="7"/>
     </row>
     <row r="165" ht="20.5" customHeight="1">
       <c r="A165" s="7"/>
       <c r="B165" s="7"/>
       <c r="C165" s="7"/>
       <c r="D165" s="7"/>
-      <c r="E165" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="F165" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="G165" s="7"/>
+      <c r="E165" t="s" s="11">
+        <v>248</v>
+      </c>
+      <c r="F165" t="s" s="12">
+        <v>249</v>
+      </c>
+      <c r="G165" s="13"/>
       <c r="H165" s="7"/>
       <c r="I165" s="7"/>
       <c r="J165" s="7"/>
-      <c r="K165" s="3"/>
+      <c r="K165" s="7"/>
     </row>
     <row r="166" ht="20.5" customHeight="1">
       <c r="A166" s="7"/>
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
       <c r="D166" s="7"/>
-      <c r="E166" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="F166" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="G166" s="7"/>
+      <c r="E166" t="s" s="11">
+        <v>250</v>
+      </c>
+      <c r="F166" t="s" s="12">
+        <v>251</v>
+      </c>
+      <c r="G166" s="13"/>
       <c r="H166" s="7"/>
       <c r="I166" s="7"/>
       <c r="J166" s="7"/>
-      <c r="K166" s="3"/>
-    </row>
-    <row r="167" ht="32.5" customHeight="1">
+      <c r="K166" s="7"/>
+    </row>
+    <row r="167" ht="20.5" customHeight="1">
       <c r="A167" s="7"/>
       <c r="B167" s="7"/>
       <c r="C167" s="7"/>
       <c r="D167" s="7"/>
-      <c r="E167" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="F167" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="G167" s="7"/>
+      <c r="E167" t="s" s="11">
+        <v>252</v>
+      </c>
+      <c r="F167" t="s" s="12">
+        <v>253</v>
+      </c>
+      <c r="G167" s="13"/>
       <c r="H167" s="7"/>
       <c r="I167" s="7"/>
       <c r="J167" s="7"/>
-      <c r="K167" s="3"/>
-    </row>
-    <row r="168" ht="32.5" customHeight="1">
+      <c r="K167" s="7"/>
+    </row>
+    <row r="168" ht="20.5" customHeight="1">
       <c r="A168" s="7"/>
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
       <c r="D168" s="7"/>
-      <c r="E168" t="s" s="2">
-        <v>241</v>
-      </c>
-      <c r="F168" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="G168" s="7"/>
+      <c r="E168" t="s" s="11">
+        <v>254</v>
+      </c>
+      <c r="F168" t="s" s="12">
+        <v>255</v>
+      </c>
+      <c r="G168" s="13"/>
       <c r="H168" s="7"/>
       <c r="I168" s="7"/>
       <c r="J168" s="7"/>
-      <c r="K168" s="3"/>
+      <c r="K168" s="7"/>
     </row>
     <row r="169" ht="20.5" customHeight="1">
       <c r="A169" s="7"/>
       <c r="B169" s="7"/>
       <c r="C169" s="7"/>
       <c r="D169" s="7"/>
-      <c r="E169" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="F169" t="s" s="2">
-        <v>244</v>
-      </c>
-      <c r="G169" s="7"/>
+      <c r="E169" t="s" s="11">
+        <v>256</v>
+      </c>
+      <c r="F169" t="s" s="12">
+        <v>257</v>
+      </c>
+      <c r="G169" s="13"/>
       <c r="H169" s="7"/>
       <c r="I169" s="7"/>
       <c r="J169" s="7"/>
-      <c r="K169" s="3"/>
-    </row>
-    <row r="170" ht="32.5" customHeight="1">
+      <c r="K169" s="7"/>
+    </row>
+    <row r="170" ht="20.5" customHeight="1">
       <c r="A170" s="7"/>
       <c r="B170" s="7"/>
       <c r="C170" s="7"/>
       <c r="D170" s="7"/>
-      <c r="E170" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="F170" t="s" s="2">
-        <v>246</v>
-      </c>
-      <c r="G170" s="7"/>
+      <c r="E170" t="s" s="11">
+        <v>258</v>
+      </c>
+      <c r="F170" t="s" s="12">
+        <v>259</v>
+      </c>
+      <c r="G170" s="13"/>
       <c r="H170" s="7"/>
       <c r="I170" s="7"/>
       <c r="J170" s="7"/>
-      <c r="K170" s="3"/>
+      <c r="K170" s="7"/>
     </row>
     <row r="171" ht="20.5" customHeight="1">
       <c r="A171" s="7"/>
       <c r="B171" s="7"/>
       <c r="C171" s="7"/>
       <c r="D171" s="7"/>
-      <c r="E171" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="F171" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="G171" s="7"/>
+      <c r="E171" t="s" s="11">
+        <v>260</v>
+      </c>
+      <c r="F171" t="s" s="12">
+        <v>261</v>
+      </c>
+      <c r="G171" s="13"/>
       <c r="H171" s="7"/>
       <c r="I171" s="7"/>
       <c r="J171" s="7"/>
-      <c r="K171" s="3"/>
+      <c r="K171" s="7"/>
     </row>
     <row r="172" ht="20.5" customHeight="1">
       <c r="A172" s="7"/>
       <c r="B172" s="7"/>
       <c r="C172" s="7"/>
       <c r="D172" s="7"/>
-      <c r="E172" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="F172" t="s" s="2">
-        <v>250</v>
-      </c>
-      <c r="G172" s="7"/>
+      <c r="E172" t="s" s="11">
+        <v>262</v>
+      </c>
+      <c r="F172" t="s" s="12">
+        <v>263</v>
+      </c>
+      <c r="G172" s="13"/>
       <c r="H172" s="7"/>
       <c r="I172" s="7"/>
       <c r="J172" s="7"/>
-      <c r="K172" s="3"/>
+      <c r="K172" s="7"/>
     </row>
     <row r="173" ht="20.5" customHeight="1">
       <c r="A173" s="7"/>
       <c r="B173" s="7"/>
       <c r="C173" s="7"/>
       <c r="D173" s="7"/>
-      <c r="E173" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="F173" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="G173" s="7"/>
+      <c r="E173" t="s" s="11">
+        <v>264</v>
+      </c>
+      <c r="F173" t="s" s="12">
+        <v>265</v>
+      </c>
+      <c r="G173" s="13"/>
       <c r="H173" s="7"/>
       <c r="I173" s="7"/>
       <c r="J173" s="7"/>
-      <c r="K173" s="3"/>
+      <c r="K173" s="7"/>
     </row>
     <row r="174" ht="20.5" customHeight="1">
       <c r="A174" s="7"/>
       <c r="B174" s="7"/>
       <c r="C174" s="7"/>
       <c r="D174" s="7"/>
-      <c r="E174" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="F174" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="G174" s="7"/>
+      <c r="E174" t="s" s="11">
+        <v>266</v>
+      </c>
+      <c r="F174" t="s" s="12">
+        <v>267</v>
+      </c>
+      <c r="G174" s="13"/>
       <c r="H174" s="7"/>
       <c r="I174" s="7"/>
       <c r="J174" s="7"/>
-      <c r="K174" s="3"/>
+      <c r="K174" s="7"/>
     </row>
     <row r="175" ht="20.5" customHeight="1">
       <c r="A175" s="7"/>
       <c r="B175" s="7"/>
       <c r="C175" s="7"/>
       <c r="D175" s="7"/>
-      <c r="E175" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="F175" t="s" s="2">
-        <v>255</v>
-      </c>
+      <c r="E175" s="7"/>
+      <c r="F175" s="14"/>
       <c r="G175" s="7"/>
       <c r="H175" s="7"/>
       <c r="I175" s="7"/>
       <c r="J175" s="7"/>
-      <c r="K175" s="3"/>
-    </row>
-    <row r="176" ht="32.5" customHeight="1">
+      <c r="K175" s="7"/>
+    </row>
+    <row r="176" ht="44.5" customHeight="1">
       <c r="A176" t="s" s="2">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="B176" t="s" s="2">
-        <v>226</v>
+        <v>269</v>
       </c>
       <c r="C176" t="s" s="2">
-        <v>257</v>
+        <v>270</v>
       </c>
       <c r="D176" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="E176" s="7"/>
-      <c r="F176" s="7"/>
+        <v>271</v>
+      </c>
+      <c r="E176" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="F176" t="s" s="2">
+        <v>273</v>
+      </c>
       <c r="G176" s="3"/>
       <c r="H176" s="3"/>
       <c r="I176" s="3"/>
       <c r="J176" s="3"/>
-      <c r="K176" s="7"/>
+      <c r="K176" s="3"/>
     </row>
     <row r="177" ht="20.5" customHeight="1">
       <c r="A177" s="7"/>
       <c r="B177" s="7"/>
       <c r="C177" s="7"/>
       <c r="D177" s="7"/>
-      <c r="E177" s="7"/>
+      <c r="E177" t="s" s="2">
+        <v>274</v>
+      </c>
       <c r="F177" s="7"/>
       <c r="G177" s="7"/>
       <c r="H177" s="7"/>
       <c r="I177" s="7"/>
       <c r="J177" s="7"/>
-      <c r="K177" s="7"/>
-    </row>
-    <row r="178" ht="32.5" customHeight="1">
+      <c r="K177" s="3"/>
+    </row>
+    <row r="178" ht="164.5" customHeight="1">
       <c r="A178" t="s" s="2">
-        <v>258</v>
+        <v>275</v>
       </c>
       <c r="B178" t="s" s="2">
-        <v>226</v>
+        <v>269</v>
       </c>
       <c r="C178" t="s" s="2">
-        <v>259</v>
+        <v>276</v>
       </c>
       <c r="D178" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="E178" s="7"/>
-      <c r="F178" s="7"/>
+        <v>271</v>
+      </c>
+      <c r="E178" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="F178" t="s" s="2">
+        <v>277</v>
+      </c>
       <c r="G178" s="3"/>
       <c r="H178" s="3"/>
       <c r="I178" s="3"/>
       <c r="J178" s="3"/>
-      <c r="K178" s="7"/>
+      <c r="K178" s="3"/>
     </row>
     <row r="179" ht="20.5" customHeight="1">
       <c r="A179" s="7"/>
@@ -7216,80 +7478,80 @@
       <c r="J179" s="7"/>
       <c r="K179" s="7"/>
     </row>
-    <row r="180" ht="32.5" customHeight="1">
-      <c r="A180" t="s" s="2">
-        <v>260</v>
-      </c>
-      <c r="B180" t="s" s="2">
-        <v>261</v>
-      </c>
-      <c r="C180" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="D180" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="E180" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="F180" t="s" s="2">
-        <v>263</v>
-      </c>
-      <c r="G180" s="3"/>
-      <c r="H180" s="3"/>
-      <c r="I180" s="3"/>
-      <c r="J180" s="3"/>
-      <c r="K180" s="3"/>
-    </row>
-    <row r="181" ht="44.5" customHeight="1">
-      <c r="A181" s="7"/>
-      <c r="B181" s="7"/>
-      <c r="C181" s="7"/>
-      <c r="D181" s="7"/>
+    <row r="180" ht="20.5" customHeight="1">
+      <c r="A180" s="7"/>
+      <c r="B180" s="7"/>
+      <c r="C180" s="7"/>
+      <c r="D180" s="7"/>
+      <c r="E180" s="7"/>
+      <c r="F180" s="7"/>
+      <c r="G180" s="7"/>
+      <c r="H180" s="7"/>
+      <c r="I180" s="7"/>
+      <c r="J180" s="7"/>
+      <c r="K180" s="7"/>
+    </row>
+    <row r="181" ht="164.5" customHeight="1">
+      <c r="A181" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="B181" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="C181" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="D181" t="s" s="2">
+        <v>271</v>
+      </c>
       <c r="E181" t="s" s="2">
-        <v>206</v>
+        <v>272</v>
       </c>
       <c r="F181" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="G181" s="7"/>
-      <c r="H181" s="7"/>
-      <c r="I181" s="7"/>
-      <c r="J181" s="7"/>
+        <v>280</v>
+      </c>
+      <c r="G181" s="3"/>
+      <c r="H181" s="3"/>
+      <c r="I181" s="3"/>
+      <c r="J181" s="3"/>
       <c r="K181" s="3"/>
     </row>
-    <row r="182" ht="44.5" customHeight="1">
+    <row r="182" ht="20.5" customHeight="1">
       <c r="A182" s="7"/>
       <c r="B182" s="7"/>
       <c r="C182" s="7"/>
       <c r="D182" s="7"/>
-      <c r="E182" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="F182" t="s" s="2">
-        <v>265</v>
-      </c>
+      <c r="E182" s="7"/>
+      <c r="F182" s="7"/>
       <c r="G182" s="7"/>
       <c r="H182" s="7"/>
       <c r="I182" s="7"/>
       <c r="J182" s="7"/>
-      <c r="K182" s="3"/>
-    </row>
-    <row r="183" ht="44.5" customHeight="1">
-      <c r="A183" s="7"/>
-      <c r="B183" s="7"/>
-      <c r="C183" s="7"/>
-      <c r="D183" s="7"/>
+      <c r="K182" s="7"/>
+    </row>
+    <row r="183" ht="20.5" customHeight="1">
+      <c r="A183" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="B183" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="C183" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="D183" t="s" s="2">
+        <v>271</v>
+      </c>
       <c r="E183" t="s" s="2">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="F183" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="G183" s="7"/>
-      <c r="H183" s="7"/>
-      <c r="I183" s="7"/>
-      <c r="J183" s="7"/>
+        <v>283</v>
+      </c>
+      <c r="G183" s="3"/>
+      <c r="H183" s="3"/>
+      <c r="I183" s="3"/>
+      <c r="J183" s="3"/>
       <c r="K183" s="3"/>
     </row>
     <row r="184" ht="20.5" customHeight="1">
@@ -7298,10 +7560,10 @@
       <c r="C184" s="7"/>
       <c r="D184" s="7"/>
       <c r="E184" t="s" s="2">
-        <v>235</v>
+        <v>274</v>
       </c>
       <c r="F184" t="s" s="2">
-        <v>267</v>
+        <v>284</v>
       </c>
       <c r="G184" s="7"/>
       <c r="H184" s="7"/>
@@ -7310,38 +7572,512 @@
       <c r="K184" s="3"/>
     </row>
     <row r="185" ht="20.5" customHeight="1">
-      <c r="A185" s="7"/>
-      <c r="B185" s="7"/>
-      <c r="C185" s="7"/>
-      <c r="D185" s="7"/>
+      <c r="A185" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="B185" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="C185" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="D185" t="s" s="2">
+        <v>271</v>
+      </c>
       <c r="E185" t="s" s="2">
-        <v>237</v>
+        <v>272</v>
       </c>
       <c r="F185" t="s" s="2">
-        <v>268</v>
-      </c>
-      <c r="G185" s="7"/>
-      <c r="H185" s="7"/>
-      <c r="I185" s="7"/>
-      <c r="J185" s="7"/>
+        <v>288</v>
+      </c>
+      <c r="G185" s="3"/>
+      <c r="H185" s="3"/>
+      <c r="I185" s="3"/>
+      <c r="J185" s="3"/>
       <c r="K185" s="3"/>
     </row>
-    <row r="186" ht="20.5" customHeight="1">
-      <c r="A186" s="7"/>
-      <c r="B186" s="7"/>
-      <c r="C186" s="7"/>
-      <c r="D186" s="7"/>
+    <row r="186" ht="116.5" customHeight="1">
+      <c r="A186" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="B186" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="C186" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="D186" t="s" s="2">
+        <v>291</v>
+      </c>
       <c r="E186" t="s" s="2">
-        <v>239</v>
+        <v>272</v>
       </c>
       <c r="F186" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="G186" s="7"/>
-      <c r="H186" s="7"/>
-      <c r="I186" s="7"/>
-      <c r="J186" s="7"/>
+        <v>292</v>
+      </c>
+      <c r="G186" s="3"/>
+      <c r="H186" s="3"/>
+      <c r="I186" s="3"/>
+      <c r="J186" s="3"/>
       <c r="K186" s="3"/>
+    </row>
+    <row r="187" ht="32.5" customHeight="1">
+      <c r="A187" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="B187" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="C187" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="D187" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="E187" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="F187" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="G187" s="3"/>
+      <c r="H187" s="3"/>
+      <c r="I187" s="3"/>
+      <c r="J187" s="3"/>
+      <c r="K187" s="3"/>
+    </row>
+    <row r="188" ht="32.5" customHeight="1">
+      <c r="A188" s="7"/>
+      <c r="B188" s="7"/>
+      <c r="C188" s="7"/>
+      <c r="D188" s="7"/>
+      <c r="E188" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="F188" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="G188" s="7"/>
+      <c r="H188" s="7"/>
+      <c r="I188" s="7"/>
+      <c r="J188" s="7"/>
+      <c r="K188" s="3"/>
+    </row>
+    <row r="189" ht="20.5" customHeight="1">
+      <c r="A189" s="7"/>
+      <c r="B189" s="7"/>
+      <c r="C189" s="7"/>
+      <c r="D189" s="7"/>
+      <c r="E189" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="F189" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="G189" s="7"/>
+      <c r="H189" s="7"/>
+      <c r="I189" s="7"/>
+      <c r="J189" s="7"/>
+      <c r="K189" s="3"/>
+    </row>
+    <row r="190" ht="20.5" customHeight="1">
+      <c r="A190" s="7"/>
+      <c r="B190" s="7"/>
+      <c r="C190" s="7"/>
+      <c r="D190" s="7"/>
+      <c r="E190" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="F190" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="G190" s="7"/>
+      <c r="H190" s="7"/>
+      <c r="I190" s="7"/>
+      <c r="J190" s="7"/>
+      <c r="K190" s="3"/>
+    </row>
+    <row r="191" ht="20.5" customHeight="1">
+      <c r="A191" s="7"/>
+      <c r="B191" s="7"/>
+      <c r="C191" s="7"/>
+      <c r="D191" s="7"/>
+      <c r="E191" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="F191" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="G191" s="7"/>
+      <c r="H191" s="7"/>
+      <c r="I191" s="7"/>
+      <c r="J191" s="7"/>
+      <c r="K191" s="3"/>
+    </row>
+    <row r="192" ht="20.5" customHeight="1">
+      <c r="A192" s="7"/>
+      <c r="B192" s="7"/>
+      <c r="C192" s="7"/>
+      <c r="D192" s="7"/>
+      <c r="E192" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="F192" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="G192" s="7"/>
+      <c r="H192" s="7"/>
+      <c r="I192" s="7"/>
+      <c r="J192" s="7"/>
+      <c r="K192" s="3"/>
+    </row>
+    <row r="193" ht="32.5" customHeight="1">
+      <c r="A193" s="7"/>
+      <c r="B193" s="7"/>
+      <c r="C193" s="7"/>
+      <c r="D193" s="7"/>
+      <c r="E193" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="F193" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="G193" s="7"/>
+      <c r="H193" s="7"/>
+      <c r="I193" s="7"/>
+      <c r="J193" s="7"/>
+      <c r="K193" s="3"/>
+    </row>
+    <row r="194" ht="32.5" customHeight="1">
+      <c r="A194" s="7"/>
+      <c r="B194" s="7"/>
+      <c r="C194" s="7"/>
+      <c r="D194" s="7"/>
+      <c r="E194" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="F194" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="G194" s="7"/>
+      <c r="H194" s="7"/>
+      <c r="I194" s="7"/>
+      <c r="J194" s="7"/>
+      <c r="K194" s="3"/>
+    </row>
+    <row r="195" ht="20.5" customHeight="1">
+      <c r="A195" s="7"/>
+      <c r="B195" s="7"/>
+      <c r="C195" s="7"/>
+      <c r="D195" s="7"/>
+      <c r="E195" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="F195" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="G195" s="7"/>
+      <c r="H195" s="7"/>
+      <c r="I195" s="7"/>
+      <c r="J195" s="7"/>
+      <c r="K195" s="3"/>
+    </row>
+    <row r="196" ht="32.5" customHeight="1">
+      <c r="A196" s="7"/>
+      <c r="B196" s="7"/>
+      <c r="C196" s="7"/>
+      <c r="D196" s="7"/>
+      <c r="E196" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="F196" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="G196" s="7"/>
+      <c r="H196" s="7"/>
+      <c r="I196" s="7"/>
+      <c r="J196" s="7"/>
+      <c r="K196" s="3"/>
+    </row>
+    <row r="197" ht="20.5" customHeight="1">
+      <c r="A197" s="7"/>
+      <c r="B197" s="7"/>
+      <c r="C197" s="7"/>
+      <c r="D197" s="7"/>
+      <c r="E197" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="F197" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="G197" s="7"/>
+      <c r="H197" s="7"/>
+      <c r="I197" s="7"/>
+      <c r="J197" s="7"/>
+      <c r="K197" s="3"/>
+    </row>
+    <row r="198" ht="20.5" customHeight="1">
+      <c r="A198" s="7"/>
+      <c r="B198" s="7"/>
+      <c r="C198" s="7"/>
+      <c r="D198" s="7"/>
+      <c r="E198" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="F198" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="G198" s="7"/>
+      <c r="H198" s="7"/>
+      <c r="I198" s="7"/>
+      <c r="J198" s="7"/>
+      <c r="K198" s="3"/>
+    </row>
+    <row r="199" ht="20.5" customHeight="1">
+      <c r="A199" s="7"/>
+      <c r="B199" s="7"/>
+      <c r="C199" s="7"/>
+      <c r="D199" s="7"/>
+      <c r="E199" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="F199" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="G199" s="7"/>
+      <c r="H199" s="7"/>
+      <c r="I199" s="7"/>
+      <c r="J199" s="7"/>
+      <c r="K199" s="3"/>
+    </row>
+    <row r="200" ht="20.5" customHeight="1">
+      <c r="A200" s="7"/>
+      <c r="B200" s="7"/>
+      <c r="C200" s="7"/>
+      <c r="D200" s="7"/>
+      <c r="E200" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="F200" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="G200" s="7"/>
+      <c r="H200" s="7"/>
+      <c r="I200" s="7"/>
+      <c r="J200" s="7"/>
+      <c r="K200" s="3"/>
+    </row>
+    <row r="201" ht="20.5" customHeight="1">
+      <c r="A201" s="7"/>
+      <c r="B201" s="7"/>
+      <c r="C201" s="7"/>
+      <c r="D201" s="7"/>
+      <c r="E201" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="F201" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="G201" s="7"/>
+      <c r="H201" s="7"/>
+      <c r="I201" s="7"/>
+      <c r="J201" s="7"/>
+      <c r="K201" s="3"/>
+    </row>
+    <row r="202" ht="32.5" customHeight="1">
+      <c r="A202" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="B202" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="C202" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="D202" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="E202" s="7"/>
+      <c r="F202" s="7"/>
+      <c r="G202" s="3"/>
+      <c r="H202" s="3"/>
+      <c r="I202" s="3"/>
+      <c r="J202" s="3"/>
+      <c r="K202" s="7"/>
+    </row>
+    <row r="203" ht="20.5" customHeight="1">
+      <c r="A203" s="7"/>
+      <c r="B203" s="7"/>
+      <c r="C203" s="7"/>
+      <c r="D203" s="7"/>
+      <c r="E203" s="7"/>
+      <c r="F203" s="7"/>
+      <c r="G203" s="7"/>
+      <c r="H203" s="7"/>
+      <c r="I203" s="7"/>
+      <c r="J203" s="7"/>
+      <c r="K203" s="7"/>
+    </row>
+    <row r="204" ht="32.5" customHeight="1">
+      <c r="A204" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="B204" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="C204" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="D204" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="E204" s="7"/>
+      <c r="F204" s="7"/>
+      <c r="G204" s="3"/>
+      <c r="H204" s="3"/>
+      <c r="I204" s="3"/>
+      <c r="J204" s="3"/>
+      <c r="K204" s="7"/>
+    </row>
+    <row r="205" ht="20.5" customHeight="1">
+      <c r="A205" s="7"/>
+      <c r="B205" s="7"/>
+      <c r="C205" s="7"/>
+      <c r="D205" s="7"/>
+      <c r="E205" s="7"/>
+      <c r="F205" s="7"/>
+      <c r="G205" s="7"/>
+      <c r="H205" s="7"/>
+      <c r="I205" s="7"/>
+      <c r="J205" s="7"/>
+      <c r="K205" s="7"/>
+    </row>
+    <row r="206" ht="32.5" customHeight="1">
+      <c r="A206" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="B206" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="C206" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="D206" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="E206" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="F206" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="G206" s="3"/>
+      <c r="H206" s="3"/>
+      <c r="I206" s="3"/>
+      <c r="J206" s="3"/>
+      <c r="K206" s="3"/>
+    </row>
+    <row r="207" ht="44.5" customHeight="1">
+      <c r="A207" s="7"/>
+      <c r="B207" s="7"/>
+      <c r="C207" s="7"/>
+      <c r="D207" s="7"/>
+      <c r="E207" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="F207" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="G207" s="7"/>
+      <c r="H207" s="7"/>
+      <c r="I207" s="7"/>
+      <c r="J207" s="7"/>
+      <c r="K207" s="3"/>
+    </row>
+    <row r="208" ht="44.5" customHeight="1">
+      <c r="A208" s="7"/>
+      <c r="B208" s="7"/>
+      <c r="C208" s="7"/>
+      <c r="D208" s="7"/>
+      <c r="E208" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="F208" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="G208" s="7"/>
+      <c r="H208" s="7"/>
+      <c r="I208" s="7"/>
+      <c r="J208" s="7"/>
+      <c r="K208" s="3"/>
+    </row>
+    <row r="209" ht="44.5" customHeight="1">
+      <c r="A209" s="7"/>
+      <c r="B209" s="7"/>
+      <c r="C209" s="7"/>
+      <c r="D209" s="7"/>
+      <c r="E209" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="F209" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="G209" s="7"/>
+      <c r="H209" s="7"/>
+      <c r="I209" s="7"/>
+      <c r="J209" s="7"/>
+      <c r="K209" s="3"/>
+    </row>
+    <row r="210" ht="20.5" customHeight="1">
+      <c r="A210" s="7"/>
+      <c r="B210" s="7"/>
+      <c r="C210" s="7"/>
+      <c r="D210" s="7"/>
+      <c r="E210" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="F210" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="G210" s="7"/>
+      <c r="H210" s="7"/>
+      <c r="I210" s="7"/>
+      <c r="J210" s="7"/>
+      <c r="K210" s="3"/>
+    </row>
+    <row r="211" ht="20.5" customHeight="1">
+      <c r="A211" s="7"/>
+      <c r="B211" s="7"/>
+      <c r="C211" s="7"/>
+      <c r="D211" s="7"/>
+      <c r="E211" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="F211" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="G211" s="7"/>
+      <c r="H211" s="7"/>
+      <c r="I211" s="7"/>
+      <c r="J211" s="7"/>
+      <c r="K211" s="3"/>
+    </row>
+    <row r="212" ht="20.5" customHeight="1">
+      <c r="A212" s="7"/>
+      <c r="B212" s="7"/>
+      <c r="C212" s="7"/>
+      <c r="D212" s="7"/>
+      <c r="E212" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="F212" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="G212" s="7"/>
+      <c r="H212" s="7"/>
+      <c r="I212" s="7"/>
+      <c r="J212" s="7"/>
+      <c r="K212" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Add a rails task that exports survey #15 into excel
15 is hard-coded because it's a known good one on my system. Could be
anything.
</commit_message>
<xml_diff>
--- a/data/Data Dictionary.xlsx
+++ b/data/Data Dictionary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="371">
   <si>
     <r>
       <rPr>
@@ -2278,14 +2278,103 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>2</t>
-    </r>
+    <t>2</t>
+  </si>
+  <si>
+    <t>IHR Coordination, Communication and Advocacy and Reporting</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Antimicrobial Resistance</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Zoonotic Disease</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Food Safety</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Immunization</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>National Laboratory System</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Biosafety and Biosecurity</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Human Resources</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Emergency Preparedness</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Emergency Response Operations</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Linking Public Health and Security Authorities</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Medical Countermeasures and Personnel Deployment</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Risk Communication</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Points of Entry</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Chemical Events</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Radiation Emergencies</t>
   </si>
   <si>
     <r>
@@ -2402,6 +2491,16 @@
         <rFont val="Calibri"/>
       </rPr>
       <t>No capacity</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>2</t>
     </r>
   </si>
   <si>
@@ -3206,15 +3305,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1210856</xdr:colOff>
+      <xdr:colOff>1191806</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>329488</xdr:rowOff>
+      <xdr:rowOff>310435</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>245656</xdr:colOff>
+      <xdr:colOff>226606</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>621588</xdr:rowOff>
+      <xdr:rowOff>602535</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3223,7 +3322,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11167656" y="39885543"/>
+          <a:off x="11148606" y="39866490"/>
           <a:ext cx="1524001" cy="292101"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4367,7 +4466,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K212"/>
+  <dimension ref="A1:K229"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -7433,36 +7532,30 @@
       <c r="E177" t="s" s="2">
         <v>274</v>
       </c>
-      <c r="F177" s="7"/>
+      <c r="F177" t="s" s="9">
+        <v>275</v>
+      </c>
       <c r="G177" s="7"/>
       <c r="H177" s="7"/>
       <c r="I177" s="7"/>
       <c r="J177" s="7"/>
       <c r="K177" s="3"/>
     </row>
-    <row r="178" ht="164.5" customHeight="1">
-      <c r="A178" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="B178" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="C178" t="s" s="2">
+    <row r="178" ht="20.5" customHeight="1">
+      <c r="A178" s="7"/>
+      <c r="B178" s="7"/>
+      <c r="C178" s="7"/>
+      <c r="D178" s="7"/>
+      <c r="E178" t="s" s="2">
         <v>276</v>
       </c>
-      <c r="D178" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="E178" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="F178" t="s" s="2">
+      <c r="F178" t="s" s="9">
         <v>277</v>
       </c>
-      <c r="G178" s="3"/>
-      <c r="H178" s="3"/>
-      <c r="I178" s="3"/>
-      <c r="J178" s="3"/>
+      <c r="G178" s="7"/>
+      <c r="H178" s="7"/>
+      <c r="I178" s="7"/>
+      <c r="J178" s="7"/>
       <c r="K178" s="3"/>
     </row>
     <row r="179" ht="20.5" customHeight="1">
@@ -7470,50 +7563,50 @@
       <c r="B179" s="7"/>
       <c r="C179" s="7"/>
       <c r="D179" s="7"/>
-      <c r="E179" s="7"/>
-      <c r="F179" s="7"/>
+      <c r="E179" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="F179" t="s" s="9">
+        <v>279</v>
+      </c>
       <c r="G179" s="7"/>
       <c r="H179" s="7"/>
       <c r="I179" s="7"/>
       <c r="J179" s="7"/>
-      <c r="K179" s="7"/>
+      <c r="K179" s="3"/>
     </row>
     <row r="180" ht="20.5" customHeight="1">
       <c r="A180" s="7"/>
       <c r="B180" s="7"/>
       <c r="C180" s="7"/>
       <c r="D180" s="7"/>
-      <c r="E180" s="7"/>
-      <c r="F180" s="7"/>
+      <c r="E180" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="F180" t="s" s="9">
+        <v>281</v>
+      </c>
       <c r="G180" s="7"/>
       <c r="H180" s="7"/>
       <c r="I180" s="7"/>
       <c r="J180" s="7"/>
-      <c r="K180" s="7"/>
-    </row>
-    <row r="181" ht="164.5" customHeight="1">
-      <c r="A181" t="s" s="2">
-        <v>278</v>
-      </c>
-      <c r="B181" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="C181" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="D181" t="s" s="2">
-        <v>271</v>
-      </c>
+      <c r="K180" s="3"/>
+    </row>
+    <row r="181" ht="20.5" customHeight="1">
+      <c r="A181" s="7"/>
+      <c r="B181" s="7"/>
+      <c r="C181" s="7"/>
+      <c r="D181" s="7"/>
       <c r="E181" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="F181" t="s" s="2">
-        <v>280</v>
-      </c>
-      <c r="G181" s="3"/>
-      <c r="H181" s="3"/>
-      <c r="I181" s="3"/>
-      <c r="J181" s="3"/>
+        <v>282</v>
+      </c>
+      <c r="F181" t="s" s="9">
+        <v>283</v>
+      </c>
+      <c r="G181" s="7"/>
+      <c r="H181" s="7"/>
+      <c r="I181" s="7"/>
+      <c r="J181" s="7"/>
       <c r="K181" s="3"/>
     </row>
     <row r="182" ht="20.5" customHeight="1">
@@ -7521,37 +7614,33 @@
       <c r="B182" s="7"/>
       <c r="C182" s="7"/>
       <c r="D182" s="7"/>
-      <c r="E182" s="7"/>
-      <c r="F182" s="7"/>
+      <c r="E182" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="F182" t="s" s="9">
+        <v>285</v>
+      </c>
       <c r="G182" s="7"/>
       <c r="H182" s="7"/>
       <c r="I182" s="7"/>
       <c r="J182" s="7"/>
-      <c r="K182" s="7"/>
+      <c r="K182" s="3"/>
     </row>
     <row r="183" ht="20.5" customHeight="1">
-      <c r="A183" t="s" s="2">
-        <v>281</v>
-      </c>
-      <c r="B183" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="C183" t="s" s="2">
-        <v>282</v>
-      </c>
-      <c r="D183" t="s" s="2">
-        <v>271</v>
-      </c>
+      <c r="A183" s="7"/>
+      <c r="B183" s="7"/>
+      <c r="C183" s="7"/>
+      <c r="D183" s="7"/>
       <c r="E183" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="F183" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="G183" s="3"/>
-      <c r="H183" s="3"/>
-      <c r="I183" s="3"/>
-      <c r="J183" s="3"/>
+        <v>286</v>
+      </c>
+      <c r="F183" t="s" s="9">
+        <v>287</v>
+      </c>
+      <c r="G183" s="7"/>
+      <c r="H183" s="7"/>
+      <c r="I183" s="7"/>
+      <c r="J183" s="7"/>
       <c r="K183" s="3"/>
     </row>
     <row r="184" ht="20.5" customHeight="1">
@@ -7560,10 +7649,10 @@
       <c r="C184" s="7"/>
       <c r="D184" s="7"/>
       <c r="E184" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="F184" t="s" s="2">
-        <v>284</v>
+        <v>288</v>
+      </c>
+      <c r="F184" t="s" s="9">
+        <v>205</v>
       </c>
       <c r="G184" s="7"/>
       <c r="H184" s="7"/>
@@ -7572,90 +7661,66 @@
       <c r="K184" s="3"/>
     </row>
     <row r="185" ht="20.5" customHeight="1">
-      <c r="A185" t="s" s="2">
-        <v>285</v>
-      </c>
-      <c r="B185" t="s" s="2">
-        <v>286</v>
-      </c>
-      <c r="C185" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="D185" t="s" s="2">
-        <v>271</v>
-      </c>
+      <c r="A185" s="7"/>
+      <c r="B185" s="7"/>
+      <c r="C185" s="7"/>
+      <c r="D185" s="7"/>
       <c r="E185" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="F185" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="G185" s="3"/>
-      <c r="H185" s="3"/>
-      <c r="I185" s="3"/>
-      <c r="J185" s="3"/>
+        <v>289</v>
+      </c>
+      <c r="F185" t="s" s="9">
+        <v>290</v>
+      </c>
+      <c r="G185" s="7"/>
+      <c r="H185" s="7"/>
+      <c r="I185" s="7"/>
+      <c r="J185" s="7"/>
       <c r="K185" s="3"/>
     </row>
-    <row r="186" ht="116.5" customHeight="1">
-      <c r="A186" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="B186" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="C186" t="s" s="2">
-        <v>290</v>
-      </c>
-      <c r="D186" t="s" s="2">
+    <row r="186" ht="20.5" customHeight="1">
+      <c r="A186" s="7"/>
+      <c r="B186" s="7"/>
+      <c r="C186" s="7"/>
+      <c r="D186" s="7"/>
+      <c r="E186" t="s" s="2">
         <v>291</v>
       </c>
-      <c r="E186" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="F186" t="s" s="2">
+      <c r="F186" t="s" s="9">
         <v>292</v>
       </c>
-      <c r="G186" s="3"/>
-      <c r="H186" s="3"/>
-      <c r="I186" s="3"/>
-      <c r="J186" s="3"/>
+      <c r="G186" s="7"/>
+      <c r="H186" s="7"/>
+      <c r="I186" s="7"/>
+      <c r="J186" s="7"/>
       <c r="K186" s="3"/>
     </row>
-    <row r="187" ht="32.5" customHeight="1">
-      <c r="A187" t="s" s="2">
+    <row r="187" ht="20.5" customHeight="1">
+      <c r="A187" s="7"/>
+      <c r="B187" s="7"/>
+      <c r="C187" s="7"/>
+      <c r="D187" s="7"/>
+      <c r="E187" t="s" s="2">
         <v>293</v>
       </c>
-      <c r="B187" t="s" s="2">
+      <c r="F187" t="s" s="9">
         <v>294</v>
       </c>
-      <c r="C187" t="s" s="2">
-        <v>295</v>
-      </c>
-      <c r="D187" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="E187" t="s" s="2">
-        <v>296</v>
-      </c>
-      <c r="F187" t="s" s="2">
-        <v>297</v>
-      </c>
-      <c r="G187" s="3"/>
-      <c r="H187" s="3"/>
-      <c r="I187" s="3"/>
-      <c r="J187" s="3"/>
+      <c r="G187" s="7"/>
+      <c r="H187" s="7"/>
+      <c r="I187" s="7"/>
+      <c r="J187" s="7"/>
       <c r="K187" s="3"/>
     </row>
-    <row r="188" ht="32.5" customHeight="1">
+    <row r="188" ht="20.5" customHeight="1">
       <c r="A188" s="7"/>
       <c r="B188" s="7"/>
       <c r="C188" s="7"/>
       <c r="D188" s="7"/>
       <c r="E188" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="F188" t="s" s="2">
-        <v>298</v>
+        <v>295</v>
+      </c>
+      <c r="F188" t="s" s="9">
+        <v>296</v>
       </c>
       <c r="G188" s="7"/>
       <c r="H188" s="7"/>
@@ -7669,10 +7734,10 @@
       <c r="C189" s="7"/>
       <c r="D189" s="7"/>
       <c r="E189" t="s" s="2">
-        <v>299</v>
-      </c>
-      <c r="F189" t="s" s="2">
-        <v>300</v>
+        <v>297</v>
+      </c>
+      <c r="F189" t="s" s="9">
+        <v>298</v>
       </c>
       <c r="G189" s="7"/>
       <c r="H189" s="7"/>
@@ -7686,10 +7751,10 @@
       <c r="C190" s="7"/>
       <c r="D190" s="7"/>
       <c r="E190" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="F190" t="s" s="2">
-        <v>302</v>
+        <v>299</v>
+      </c>
+      <c r="F190" t="s" s="9">
+        <v>300</v>
       </c>
       <c r="G190" s="7"/>
       <c r="H190" s="7"/>
@@ -7703,10 +7768,10 @@
       <c r="C191" s="7"/>
       <c r="D191" s="7"/>
       <c r="E191" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="F191" t="s" s="2">
-        <v>304</v>
+        <v>301</v>
+      </c>
+      <c r="F191" t="s" s="9">
+        <v>302</v>
       </c>
       <c r="G191" s="7"/>
       <c r="H191" s="7"/>
@@ -7720,10 +7785,10 @@
       <c r="C192" s="7"/>
       <c r="D192" s="7"/>
       <c r="E192" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="F192" t="s" s="2">
-        <v>306</v>
+        <v>303</v>
+      </c>
+      <c r="F192" t="s" s="9">
+        <v>304</v>
       </c>
       <c r="G192" s="7"/>
       <c r="H192" s="7"/>
@@ -7731,16 +7796,16 @@
       <c r="J192" s="7"/>
       <c r="K192" s="3"/>
     </row>
-    <row r="193" ht="32.5" customHeight="1">
+    <row r="193" ht="20.5" customHeight="1">
       <c r="A193" s="7"/>
       <c r="B193" s="7"/>
       <c r="C193" s="7"/>
       <c r="D193" s="7"/>
       <c r="E193" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="F193" t="s" s="2">
-        <v>308</v>
+        <v>305</v>
+      </c>
+      <c r="F193" t="s" s="9">
+        <v>306</v>
       </c>
       <c r="G193" s="7"/>
       <c r="H193" s="7"/>
@@ -7748,89 +7813,93 @@
       <c r="J193" s="7"/>
       <c r="K193" s="3"/>
     </row>
-    <row r="194" ht="32.5" customHeight="1">
+    <row r="194" ht="20.5" customHeight="1">
       <c r="A194" s="7"/>
       <c r="B194" s="7"/>
       <c r="C194" s="7"/>
       <c r="D194" s="7"/>
-      <c r="E194" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="F194" t="s" s="2">
-        <v>310</v>
-      </c>
+      <c r="E194" s="2"/>
+      <c r="F194" s="7"/>
       <c r="G194" s="7"/>
       <c r="H194" s="7"/>
       <c r="I194" s="7"/>
       <c r="J194" s="7"/>
       <c r="K194" s="3"/>
     </row>
-    <row r="195" ht="20.5" customHeight="1">
-      <c r="A195" s="7"/>
-      <c r="B195" s="7"/>
-      <c r="C195" s="7"/>
-      <c r="D195" s="7"/>
+    <row r="195" ht="164.5" customHeight="1">
+      <c r="A195" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="B195" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="C195" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="D195" t="s" s="2">
+        <v>271</v>
+      </c>
       <c r="E195" t="s" s="2">
-        <v>311</v>
+        <v>272</v>
       </c>
       <c r="F195" t="s" s="2">
-        <v>312</v>
-      </c>
-      <c r="G195" s="7"/>
-      <c r="H195" s="7"/>
-      <c r="I195" s="7"/>
-      <c r="J195" s="7"/>
+        <v>309</v>
+      </c>
+      <c r="G195" s="3"/>
+      <c r="H195" s="3"/>
+      <c r="I195" s="3"/>
+      <c r="J195" s="3"/>
       <c r="K195" s="3"/>
     </row>
-    <row r="196" ht="32.5" customHeight="1">
+    <row r="196" ht="20.5" customHeight="1">
       <c r="A196" s="7"/>
       <c r="B196" s="7"/>
       <c r="C196" s="7"/>
       <c r="D196" s="7"/>
-      <c r="E196" t="s" s="2">
-        <v>313</v>
-      </c>
-      <c r="F196" t="s" s="2">
-        <v>314</v>
-      </c>
+      <c r="E196" s="7"/>
+      <c r="F196" s="7"/>
       <c r="G196" s="7"/>
       <c r="H196" s="7"/>
       <c r="I196" s="7"/>
       <c r="J196" s="7"/>
-      <c r="K196" s="3"/>
+      <c r="K196" s="7"/>
     </row>
     <row r="197" ht="20.5" customHeight="1">
       <c r="A197" s="7"/>
       <c r="B197" s="7"/>
       <c r="C197" s="7"/>
       <c r="D197" s="7"/>
-      <c r="E197" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="F197" t="s" s="2">
-        <v>316</v>
-      </c>
+      <c r="E197" s="7"/>
+      <c r="F197" s="7"/>
       <c r="G197" s="7"/>
       <c r="H197" s="7"/>
       <c r="I197" s="7"/>
       <c r="J197" s="7"/>
-      <c r="K197" s="3"/>
-    </row>
-    <row r="198" ht="20.5" customHeight="1">
-      <c r="A198" s="7"/>
-      <c r="B198" s="7"/>
-      <c r="C198" s="7"/>
-      <c r="D198" s="7"/>
+      <c r="K197" s="7"/>
+    </row>
+    <row r="198" ht="164.5" customHeight="1">
+      <c r="A198" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="B198" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="C198" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="D198" t="s" s="2">
+        <v>271</v>
+      </c>
       <c r="E198" t="s" s="2">
-        <v>317</v>
+        <v>272</v>
       </c>
       <c r="F198" t="s" s="2">
-        <v>318</v>
-      </c>
-      <c r="G198" s="7"/>
-      <c r="H198" s="7"/>
-      <c r="I198" s="7"/>
-      <c r="J198" s="7"/>
+        <v>312</v>
+      </c>
+      <c r="G198" s="3"/>
+      <c r="H198" s="3"/>
+      <c r="I198" s="3"/>
+      <c r="J198" s="3"/>
       <c r="K198" s="3"/>
     </row>
     <row r="199" ht="20.5" customHeight="1">
@@ -7838,33 +7907,37 @@
       <c r="B199" s="7"/>
       <c r="C199" s="7"/>
       <c r="D199" s="7"/>
-      <c r="E199" t="s" s="2">
-        <v>319</v>
-      </c>
-      <c r="F199" t="s" s="2">
-        <v>27</v>
-      </c>
+      <c r="E199" s="7"/>
+      <c r="F199" s="7"/>
       <c r="G199" s="7"/>
       <c r="H199" s="7"/>
       <c r="I199" s="7"/>
       <c r="J199" s="7"/>
-      <c r="K199" s="3"/>
+      <c r="K199" s="7"/>
     </row>
     <row r="200" ht="20.5" customHeight="1">
-      <c r="A200" s="7"/>
-      <c r="B200" s="7"/>
-      <c r="C200" s="7"/>
-      <c r="D200" s="7"/>
+      <c r="A200" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="B200" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="C200" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="D200" t="s" s="2">
+        <v>271</v>
+      </c>
       <c r="E200" t="s" s="2">
-        <v>320</v>
+        <v>272</v>
       </c>
       <c r="F200" t="s" s="2">
-        <v>321</v>
-      </c>
-      <c r="G200" s="7"/>
-      <c r="H200" s="7"/>
-      <c r="I200" s="7"/>
-      <c r="J200" s="7"/>
+        <v>315</v>
+      </c>
+      <c r="G200" s="3"/>
+      <c r="H200" s="3"/>
+      <c r="I200" s="3"/>
+      <c r="J200" s="3"/>
       <c r="K200" s="3"/>
     </row>
     <row r="201" ht="20.5" customHeight="1">
@@ -7873,10 +7946,10 @@
       <c r="C201" s="7"/>
       <c r="D201" s="7"/>
       <c r="E201" t="s" s="2">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="F201" t="s" s="2">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="G201" s="7"/>
       <c r="H201" s="7"/>
@@ -7884,109 +7957,125 @@
       <c r="J201" s="7"/>
       <c r="K201" s="3"/>
     </row>
-    <row r="202" ht="32.5" customHeight="1">
+    <row r="202" ht="20.5" customHeight="1">
       <c r="A202" t="s" s="2">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="B202" t="s" s="2">
-        <v>294</v>
+        <v>319</v>
       </c>
       <c r="C202" t="s" s="2">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D202" t="s" s="2">
         <v>271</v>
       </c>
-      <c r="E202" s="7"/>
-      <c r="F202" s="7"/>
+      <c r="E202" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="F202" t="s" s="2">
+        <v>321</v>
+      </c>
       <c r="G202" s="3"/>
       <c r="H202" s="3"/>
       <c r="I202" s="3"/>
       <c r="J202" s="3"/>
-      <c r="K202" s="7"/>
-    </row>
-    <row r="203" ht="20.5" customHeight="1">
-      <c r="A203" s="7"/>
-      <c r="B203" s="7"/>
-      <c r="C203" s="7"/>
-      <c r="D203" s="7"/>
-      <c r="E203" s="7"/>
-      <c r="F203" s="7"/>
-      <c r="G203" s="7"/>
-      <c r="H203" s="7"/>
-      <c r="I203" s="7"/>
-      <c r="J203" s="7"/>
-      <c r="K203" s="7"/>
+      <c r="K202" s="3"/>
+    </row>
+    <row r="203" ht="116.5" customHeight="1">
+      <c r="A203" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="B203" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="C203" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="D203" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="E203" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="F203" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="G203" s="3"/>
+      <c r="H203" s="3"/>
+      <c r="I203" s="3"/>
+      <c r="J203" s="3"/>
+      <c r="K203" s="3"/>
     </row>
     <row r="204" ht="32.5" customHeight="1">
       <c r="A204" t="s" s="2">
         <v>326</v>
       </c>
       <c r="B204" t="s" s="2">
-        <v>294</v>
+        <v>327</v>
       </c>
       <c r="C204" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D204" t="s" s="2">
         <v>271</v>
       </c>
-      <c r="E204" s="7"/>
-      <c r="F204" s="7"/>
+      <c r="E204" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="F204" t="s" s="2">
+        <v>330</v>
+      </c>
       <c r="G204" s="3"/>
       <c r="H204" s="3"/>
       <c r="I204" s="3"/>
       <c r="J204" s="3"/>
-      <c r="K204" s="7"/>
-    </row>
-    <row r="205" ht="20.5" customHeight="1">
+      <c r="K204" s="3"/>
+    </row>
+    <row r="205" ht="32.5" customHeight="1">
       <c r="A205" s="7"/>
       <c r="B205" s="7"/>
       <c r="C205" s="7"/>
       <c r="D205" s="7"/>
-      <c r="E205" s="7"/>
-      <c r="F205" s="7"/>
+      <c r="E205" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="F205" t="s" s="2">
+        <v>331</v>
+      </c>
       <c r="G205" s="7"/>
       <c r="H205" s="7"/>
       <c r="I205" s="7"/>
       <c r="J205" s="7"/>
-      <c r="K205" s="7"/>
-    </row>
-    <row r="206" ht="32.5" customHeight="1">
-      <c r="A206" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="B206" t="s" s="2">
-        <v>329</v>
-      </c>
-      <c r="C206" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="D206" t="s" s="2">
-        <v>271</v>
-      </c>
+      <c r="K205" s="3"/>
+    </row>
+    <row r="206" ht="20.5" customHeight="1">
+      <c r="A206" s="7"/>
+      <c r="B206" s="7"/>
+      <c r="C206" s="7"/>
+      <c r="D206" s="7"/>
       <c r="E206" t="s" s="2">
-        <v>272</v>
+        <v>332</v>
       </c>
       <c r="F206" t="s" s="2">
-        <v>331</v>
-      </c>
-      <c r="G206" s="3"/>
-      <c r="H206" s="3"/>
-      <c r="I206" s="3"/>
-      <c r="J206" s="3"/>
+        <v>333</v>
+      </c>
+      <c r="G206" s="7"/>
+      <c r="H206" s="7"/>
+      <c r="I206" s="7"/>
+      <c r="J206" s="7"/>
       <c r="K206" s="3"/>
     </row>
-    <row r="207" ht="44.5" customHeight="1">
+    <row r="207" ht="20.5" customHeight="1">
       <c r="A207" s="7"/>
       <c r="B207" s="7"/>
       <c r="C207" s="7"/>
       <c r="D207" s="7"/>
       <c r="E207" t="s" s="2">
-        <v>274</v>
+        <v>334</v>
       </c>
       <c r="F207" t="s" s="2">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="G207" s="7"/>
       <c r="H207" s="7"/>
@@ -7994,16 +8083,16 @@
       <c r="J207" s="7"/>
       <c r="K207" s="3"/>
     </row>
-    <row r="208" ht="44.5" customHeight="1">
+    <row r="208" ht="20.5" customHeight="1">
       <c r="A208" s="7"/>
       <c r="B208" s="7"/>
       <c r="C208" s="7"/>
       <c r="D208" s="7"/>
       <c r="E208" t="s" s="2">
-        <v>299</v>
+        <v>336</v>
       </c>
       <c r="F208" t="s" s="2">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="G208" s="7"/>
       <c r="H208" s="7"/>
@@ -8011,16 +8100,16 @@
       <c r="J208" s="7"/>
       <c r="K208" s="3"/>
     </row>
-    <row r="209" ht="44.5" customHeight="1">
+    <row r="209" ht="20.5" customHeight="1">
       <c r="A209" s="7"/>
       <c r="B209" s="7"/>
       <c r="C209" s="7"/>
       <c r="D209" s="7"/>
       <c r="E209" t="s" s="2">
-        <v>301</v>
+        <v>338</v>
       </c>
       <c r="F209" t="s" s="2">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="G209" s="7"/>
       <c r="H209" s="7"/>
@@ -8028,16 +8117,16 @@
       <c r="J209" s="7"/>
       <c r="K209" s="3"/>
     </row>
-    <row r="210" ht="20.5" customHeight="1">
+    <row r="210" ht="32.5" customHeight="1">
       <c r="A210" s="7"/>
       <c r="B210" s="7"/>
       <c r="C210" s="7"/>
       <c r="D210" s="7"/>
       <c r="E210" t="s" s="2">
-        <v>303</v>
+        <v>340</v>
       </c>
       <c r="F210" t="s" s="2">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="G210" s="7"/>
       <c r="H210" s="7"/>
@@ -8045,16 +8134,16 @@
       <c r="J210" s="7"/>
       <c r="K210" s="3"/>
     </row>
-    <row r="211" ht="20.5" customHeight="1">
+    <row r="211" ht="32.5" customHeight="1">
       <c r="A211" s="7"/>
       <c r="B211" s="7"/>
       <c r="C211" s="7"/>
       <c r="D211" s="7"/>
       <c r="E211" t="s" s="2">
-        <v>305</v>
+        <v>342</v>
       </c>
       <c r="F211" t="s" s="2">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="G211" s="7"/>
       <c r="H211" s="7"/>
@@ -8068,16 +8157,313 @@
       <c r="C212" s="7"/>
       <c r="D212" s="7"/>
       <c r="E212" t="s" s="2">
-        <v>307</v>
+        <v>344</v>
       </c>
       <c r="F212" t="s" s="2">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="G212" s="7"/>
       <c r="H212" s="7"/>
       <c r="I212" s="7"/>
       <c r="J212" s="7"/>
       <c r="K212" s="3"/>
+    </row>
+    <row r="213" ht="32.5" customHeight="1">
+      <c r="A213" s="7"/>
+      <c r="B213" s="7"/>
+      <c r="C213" s="7"/>
+      <c r="D213" s="7"/>
+      <c r="E213" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="F213" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="G213" s="7"/>
+      <c r="H213" s="7"/>
+      <c r="I213" s="7"/>
+      <c r="J213" s="7"/>
+      <c r="K213" s="3"/>
+    </row>
+    <row r="214" ht="20.5" customHeight="1">
+      <c r="A214" s="7"/>
+      <c r="B214" s="7"/>
+      <c r="C214" s="7"/>
+      <c r="D214" s="7"/>
+      <c r="E214" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="F214" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="G214" s="7"/>
+      <c r="H214" s="7"/>
+      <c r="I214" s="7"/>
+      <c r="J214" s="7"/>
+      <c r="K214" s="3"/>
+    </row>
+    <row r="215" ht="20.5" customHeight="1">
+      <c r="A215" s="7"/>
+      <c r="B215" s="7"/>
+      <c r="C215" s="7"/>
+      <c r="D215" s="7"/>
+      <c r="E215" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="F215" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="G215" s="7"/>
+      <c r="H215" s="7"/>
+      <c r="I215" s="7"/>
+      <c r="J215" s="7"/>
+      <c r="K215" s="3"/>
+    </row>
+    <row r="216" ht="20.5" customHeight="1">
+      <c r="A216" s="7"/>
+      <c r="B216" s="7"/>
+      <c r="C216" s="7"/>
+      <c r="D216" s="7"/>
+      <c r="E216" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="F216" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="G216" s="7"/>
+      <c r="H216" s="7"/>
+      <c r="I216" s="7"/>
+      <c r="J216" s="7"/>
+      <c r="K216" s="3"/>
+    </row>
+    <row r="217" ht="20.5" customHeight="1">
+      <c r="A217" s="7"/>
+      <c r="B217" s="7"/>
+      <c r="C217" s="7"/>
+      <c r="D217" s="7"/>
+      <c r="E217" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="F217" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="G217" s="7"/>
+      <c r="H217" s="7"/>
+      <c r="I217" s="7"/>
+      <c r="J217" s="7"/>
+      <c r="K217" s="3"/>
+    </row>
+    <row r="218" ht="20.5" customHeight="1">
+      <c r="A218" s="7"/>
+      <c r="B218" s="7"/>
+      <c r="C218" s="7"/>
+      <c r="D218" s="7"/>
+      <c r="E218" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="F218" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="G218" s="7"/>
+      <c r="H218" s="7"/>
+      <c r="I218" s="7"/>
+      <c r="J218" s="7"/>
+      <c r="K218" s="3"/>
+    </row>
+    <row r="219" ht="32.5" customHeight="1">
+      <c r="A219" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="B219" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="C219" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="D219" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="E219" s="7"/>
+      <c r="F219" s="7"/>
+      <c r="G219" s="3"/>
+      <c r="H219" s="3"/>
+      <c r="I219" s="3"/>
+      <c r="J219" s="3"/>
+      <c r="K219" s="7"/>
+    </row>
+    <row r="220" ht="20.5" customHeight="1">
+      <c r="A220" s="7"/>
+      <c r="B220" s="7"/>
+      <c r="C220" s="7"/>
+      <c r="D220" s="7"/>
+      <c r="E220" s="7"/>
+      <c r="F220" s="7"/>
+      <c r="G220" s="7"/>
+      <c r="H220" s="7"/>
+      <c r="I220" s="7"/>
+      <c r="J220" s="7"/>
+      <c r="K220" s="7"/>
+    </row>
+    <row r="221" ht="32.5" customHeight="1">
+      <c r="A221" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="B221" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="C221" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="D221" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="E221" s="7"/>
+      <c r="F221" s="7"/>
+      <c r="G221" s="3"/>
+      <c r="H221" s="3"/>
+      <c r="I221" s="3"/>
+      <c r="J221" s="3"/>
+      <c r="K221" s="7"/>
+    </row>
+    <row r="222" ht="20.5" customHeight="1">
+      <c r="A222" s="7"/>
+      <c r="B222" s="7"/>
+      <c r="C222" s="7"/>
+      <c r="D222" s="7"/>
+      <c r="E222" s="7"/>
+      <c r="F222" s="7"/>
+      <c r="G222" s="7"/>
+      <c r="H222" s="7"/>
+      <c r="I222" s="7"/>
+      <c r="J222" s="7"/>
+      <c r="K222" s="7"/>
+    </row>
+    <row r="223" ht="32.5" customHeight="1">
+      <c r="A223" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="B223" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="C223" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="D223" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="E223" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="F223" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="G223" s="3"/>
+      <c r="H223" s="3"/>
+      <c r="I223" s="3"/>
+      <c r="J223" s="3"/>
+      <c r="K223" s="3"/>
+    </row>
+    <row r="224" ht="44.5" customHeight="1">
+      <c r="A224" s="7"/>
+      <c r="B224" s="7"/>
+      <c r="C224" s="7"/>
+      <c r="D224" s="7"/>
+      <c r="E224" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="F224" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="G224" s="7"/>
+      <c r="H224" s="7"/>
+      <c r="I224" s="7"/>
+      <c r="J224" s="7"/>
+      <c r="K224" s="3"/>
+    </row>
+    <row r="225" ht="44.5" customHeight="1">
+      <c r="A225" s="7"/>
+      <c r="B225" s="7"/>
+      <c r="C225" s="7"/>
+      <c r="D225" s="7"/>
+      <c r="E225" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="F225" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="G225" s="7"/>
+      <c r="H225" s="7"/>
+      <c r="I225" s="7"/>
+      <c r="J225" s="7"/>
+      <c r="K225" s="3"/>
+    </row>
+    <row r="226" ht="44.5" customHeight="1">
+      <c r="A226" s="7"/>
+      <c r="B226" s="7"/>
+      <c r="C226" s="7"/>
+      <c r="D226" s="7"/>
+      <c r="E226" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="F226" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="G226" s="7"/>
+      <c r="H226" s="7"/>
+      <c r="I226" s="7"/>
+      <c r="J226" s="7"/>
+      <c r="K226" s="3"/>
+    </row>
+    <row r="227" ht="20.5" customHeight="1">
+      <c r="A227" s="7"/>
+      <c r="B227" s="7"/>
+      <c r="C227" s="7"/>
+      <c r="D227" s="7"/>
+      <c r="E227" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="F227" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="G227" s="7"/>
+      <c r="H227" s="7"/>
+      <c r="I227" s="7"/>
+      <c r="J227" s="7"/>
+      <c r="K227" s="3"/>
+    </row>
+    <row r="228" ht="20.5" customHeight="1">
+      <c r="A228" s="7"/>
+      <c r="B228" s="7"/>
+      <c r="C228" s="7"/>
+      <c r="D228" s="7"/>
+      <c r="E228" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="F228" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="G228" s="7"/>
+      <c r="H228" s="7"/>
+      <c r="I228" s="7"/>
+      <c r="J228" s="7"/>
+      <c r="K228" s="3"/>
+    </row>
+    <row r="229" ht="20.5" customHeight="1">
+      <c r="A229" s="7"/>
+      <c r="B229" s="7"/>
+      <c r="C229" s="7"/>
+      <c r="D229" s="7"/>
+      <c r="E229" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="F229" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="G229" s="7"/>
+      <c r="H229" s="7"/>
+      <c r="I229" s="7"/>
+      <c r="J229" s="7"/>
+      <c r="K229" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>